<commit_message>
add shiny script and data
</commit_message>
<xml_diff>
--- a/01_pur1/output/PUR_unresolved_case.xlsx
+++ b/01_pur1/output/PUR_unresolved_case.xlsx
@@ -1,98 +1,105 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icrafcifor-my.sharepoint.com/personal/f_mahezs_cifor-icraf_org/Documents/Documents/GitHub/lumens-shiny/01_pur1/output/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="35" documentId="11_42CED8001B57DD8F5E9062C278C5FF6ED7EE992C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41072DE2-F741-4E00-B072-58E4F6EE0A32}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="PUR_unresolved_case" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="PUR_unresolved_case" sheetId="1" r:id="rId1"/>
     <sheet name="drop-down_attribute" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
-  <si>
-    <t xml:space="preserve">ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rec_phase1b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PU_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PU_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PU_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PU_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REFERENCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">COUNT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reconcile Action</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unresolved_case</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Perkebunan_Bungo_F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hutan Lindung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hutan_Adat_Bungo_F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HTI_Bungo_F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tambang_Bungo_F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hutan Produksi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Perkebunan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pertanian Lahan Basah</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pertanian Lahan Kering</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sempadan Sungai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Perkotaaan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taman Nasional Kerinci Sebelat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unresolved</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="24">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Rec_phase1b</t>
+  </si>
+  <si>
+    <t>PU_1</t>
+  </si>
+  <si>
+    <t>PU_2</t>
+  </si>
+  <si>
+    <t>PU_3</t>
+  </si>
+  <si>
+    <t>PU_4</t>
+  </si>
+  <si>
+    <t>REFERENCE</t>
+  </si>
+  <si>
+    <t>COUNT</t>
+  </si>
+  <si>
+    <t>Reconcile Action</t>
+  </si>
+  <si>
+    <t>unresolved_case</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Perkebunan_Bungo_F</t>
+  </si>
+  <si>
+    <t>Hutan Lindung</t>
+  </si>
+  <si>
+    <t>Hutan_Adat_Bungo_F</t>
+  </si>
+  <si>
+    <t>HTI_Bungo_F</t>
+  </si>
+  <si>
+    <t>Tambang_Bungo_F</t>
+  </si>
+  <si>
+    <t>Hutan Produksi</t>
+  </si>
+  <si>
+    <t>Perkebunan</t>
+  </si>
+  <si>
+    <t>Pertanian Lahan Basah</t>
+  </si>
+  <si>
+    <t>Pertanian Lahan Kering</t>
+  </si>
+  <si>
+    <t>Sempadan Sungai</t>
+  </si>
+  <si>
+    <t>Perkotaaan</t>
+  </si>
+  <si>
+    <t>Taman Nasional Kerinci Sebelat</t>
+  </si>
+  <si>
+    <t>unresolved</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -128,6 +135,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -409,14 +425,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="24.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -445,8 +466,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>17</v>
       </c>
       <c r="B2" t="s">
@@ -467,15 +488,15 @@
       <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2">
         <v>2513</v>
       </c>
       <c r="I2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>34</v>
       </c>
       <c r="B3" t="s">
@@ -496,15 +517,15 @@
       <c r="G3" t="s">
         <v>12</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H3">
         <v>128</v>
       </c>
       <c r="I3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>30</v>
       </c>
       <c r="B4" t="s">
@@ -525,15 +546,15 @@
       <c r="G4" t="s">
         <v>12</v>
       </c>
-      <c r="H4" t="n">
+      <c r="H4">
         <v>2095</v>
       </c>
       <c r="I4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>42</v>
       </c>
       <c r="B5" t="s">
@@ -554,15 +575,15 @@
       <c r="G5" t="s">
         <v>16</v>
       </c>
-      <c r="H5" t="n">
+      <c r="H5">
         <v>2492</v>
       </c>
       <c r="I5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>10</v>
       </c>
       <c r="B6" t="s">
@@ -583,15 +604,15 @@
       <c r="G6" t="s">
         <v>16</v>
       </c>
-      <c r="H6" t="n">
+      <c r="H6">
         <v>8828</v>
       </c>
       <c r="I6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>46</v>
       </c>
       <c r="B7" t="s">
@@ -612,15 +633,15 @@
       <c r="G7" t="s">
         <v>16</v>
       </c>
-      <c r="H7" t="n">
+      <c r="H7">
         <v>3598</v>
       </c>
       <c r="I7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>24</v>
       </c>
       <c r="B8" t="s">
@@ -641,15 +662,15 @@
       <c r="G8" t="s">
         <v>16</v>
       </c>
-      <c r="H8" t="n">
+      <c r="H8">
         <v>1906</v>
       </c>
       <c r="I8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>51</v>
       </c>
       <c r="B9" t="s">
@@ -670,15 +691,15 @@
       <c r="G9" t="s">
         <v>16</v>
       </c>
-      <c r="H9" t="n">
+      <c r="H9">
         <v>25</v>
       </c>
       <c r="I9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>54</v>
       </c>
       <c r="B10" t="s">
@@ -699,15 +720,15 @@
       <c r="G10" t="s">
         <v>16</v>
       </c>
-      <c r="H10" t="n">
+      <c r="H10">
         <v>169</v>
       </c>
       <c r="I10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>37</v>
       </c>
       <c r="B11" t="s">
@@ -728,15 +749,15 @@
       <c r="G11" t="s">
         <v>16</v>
       </c>
-      <c r="H11" t="n">
+      <c r="H11">
         <v>28784</v>
       </c>
       <c r="I11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>52</v>
       </c>
       <c r="B12" t="s">
@@ -757,15 +778,15 @@
       <c r="G12" t="s">
         <v>17</v>
       </c>
-      <c r="H12" t="n">
+      <c r="H12">
         <v>270</v>
       </c>
       <c r="I12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>47</v>
       </c>
       <c r="B13" t="s">
@@ -786,15 +807,15 @@
       <c r="G13" t="s">
         <v>17</v>
       </c>
-      <c r="H13" t="n">
+      <c r="H13">
         <v>528</v>
       </c>
       <c r="I13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>43</v>
       </c>
       <c r="B14" t="s">
@@ -815,15 +836,15 @@
       <c r="G14" t="s">
         <v>17</v>
       </c>
-      <c r="H14" t="n">
+      <c r="H14">
         <v>177</v>
       </c>
       <c r="I14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>25</v>
       </c>
       <c r="B15" t="s">
@@ -844,15 +865,15 @@
       <c r="G15" t="s">
         <v>17</v>
       </c>
-      <c r="H15" t="n">
+      <c r="H15">
         <v>8687</v>
       </c>
       <c r="I15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>38</v>
       </c>
       <c r="B16" t="s">
@@ -873,15 +894,15 @@
       <c r="G16" t="s">
         <v>17</v>
       </c>
-      <c r="H16" t="n">
+      <c r="H16">
         <v>142</v>
       </c>
       <c r="I16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>11</v>
       </c>
       <c r="B17" t="s">
@@ -902,15 +923,15 @@
       <c r="G17" t="s">
         <v>17</v>
       </c>
-      <c r="H17" t="n">
+      <c r="H17">
         <v>5392</v>
       </c>
       <c r="I17" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>44</v>
       </c>
       <c r="B18" t="s">
@@ -931,15 +952,15 @@
       <c r="G18" t="s">
         <v>18</v>
       </c>
-      <c r="H18" t="n">
+      <c r="H18">
         <v>1179</v>
       </c>
       <c r="I18" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>39</v>
       </c>
       <c r="B19" t="s">
@@ -960,15 +981,15 @@
       <c r="G19" t="s">
         <v>18</v>
       </c>
-      <c r="H19" t="n">
+      <c r="H19">
         <v>2036</v>
       </c>
       <c r="I19" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
         <v>27</v>
       </c>
       <c r="B20" t="s">
@@ -989,15 +1010,15 @@
       <c r="G20" t="s">
         <v>18</v>
       </c>
-      <c r="H20" t="n">
+      <c r="H20">
         <v>3449</v>
       </c>
       <c r="I20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>53</v>
       </c>
       <c r="B21" t="s">
@@ -1018,15 +1039,15 @@
       <c r="G21" t="s">
         <v>18</v>
       </c>
-      <c r="H21" t="n">
+      <c r="H21">
         <v>111</v>
       </c>
       <c r="I21" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
         <v>48</v>
       </c>
       <c r="B22" t="s">
@@ -1047,15 +1068,15 @@
       <c r="G22" t="s">
         <v>18</v>
       </c>
-      <c r="H22" t="n">
+      <c r="H22">
         <v>25</v>
       </c>
       <c r="I22" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
         <v>13</v>
       </c>
       <c r="B23" t="s">
@@ -1076,15 +1097,15 @@
       <c r="G23" t="s">
         <v>18</v>
       </c>
-      <c r="H23" t="n">
+      <c r="H23">
         <v>6290</v>
       </c>
       <c r="I23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>28</v>
       </c>
       <c r="B24" t="s">
@@ -1105,15 +1126,15 @@
       <c r="G24" t="s">
         <v>19</v>
       </c>
-      <c r="H24" t="n">
+      <c r="H24">
         <v>3960</v>
       </c>
       <c r="I24" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>49</v>
       </c>
       <c r="B25" t="s">
@@ -1134,15 +1155,15 @@
       <c r="G25" t="s">
         <v>19</v>
       </c>
-      <c r="H25" t="n">
+      <c r="H25">
         <v>3</v>
       </c>
       <c r="I25" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
         <v>14</v>
       </c>
       <c r="B26" t="s">
@@ -1163,15 +1184,15 @@
       <c r="G26" t="s">
         <v>19</v>
       </c>
-      <c r="H26" t="n">
+      <c r="H26">
         <v>4093</v>
       </c>
       <c r="I26" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>29</v>
       </c>
       <c r="B27" t="s">
@@ -1192,15 +1213,15 @@
       <c r="G27" t="s">
         <v>20</v>
       </c>
-      <c r="H27" t="n">
+      <c r="H27">
         <v>466</v>
       </c>
       <c r="I27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
         <v>33</v>
       </c>
       <c r="B28" t="s">
@@ -1221,15 +1242,15 @@
       <c r="G28" t="s">
         <v>20</v>
       </c>
-      <c r="H28" t="n">
+      <c r="H28">
         <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>50</v>
       </c>
       <c r="B29" t="s">
@@ -1250,15 +1271,15 @@
       <c r="G29" t="s">
         <v>20</v>
       </c>
-      <c r="H29" t="n">
+      <c r="H29">
         <v>79</v>
       </c>
       <c r="I29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>23</v>
       </c>
       <c r="B30" t="s">
@@ -1279,20 +1300,20 @@
       <c r="G30" t="s">
         <v>20</v>
       </c>
-      <c r="H30" t="n">
+      <c r="H30">
         <v>2230</v>
       </c>
       <c r="I30" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>'drop-down_attribute'!$A$2:$A$15</xm:f>
           </x14:formula1>
@@ -1305,90 +1326,90 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update on ui shiny; add help file
</commit_message>
<xml_diff>
--- a/01_pur1/output/PUR_unresolved_case.xlsx
+++ b/01_pur1/output/PUR_unresolved_case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icrafcifor-my.sharepoint.com/personal/f_mahezs_cifor-icraf_org/Documents/Documents/GitHub/lumens-shiny/01_pur1/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="35" documentId="11_42CED8001B57DD8F5E9062C278C5FF6ED7EE992C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41072DE2-F741-4E00-B072-58E4F6EE0A32}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="11_42CED8001B57DD8F5E9062C278C5FF6ED7EE992C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE37223F-BC3B-4941-82EA-87F65D2C213A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -429,7 +429,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,7 +579,7 @@
         <v>2492</v>
       </c>
       <c r="I5" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
improve quick user guide
</commit_message>
<xml_diff>
--- a/01_pur1/output/PUR_unresolved_case.xlsx
+++ b/01_pur1/output/PUR_unresolved_case.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -429,7 +429,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>